<commit_message>
Made new 'Note' class
added new note class to have more properties such as sound and an image file
</commit_message>
<xml_diff>
--- a/flowcharts/MIDI_controller_charts.xlsx
+++ b/flowcharts/MIDI_controller_charts.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Repositories\Flute_Learning_Program\flowcharts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13EDD55F-D2EE-4D1B-9A81-CAE3E4895480}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21A616E2-7B71-40D1-BA63-0313D3496102}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{0C41BF42-A1AE-4A73-8224-13896CE221AE}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{0C41BF42-A1AE-4A73-8224-13896CE221AE}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Button sheet" sheetId="2" r:id="rId2"/>
+    <sheet name="Old Stuff" sheetId="1" r:id="rId1"/>
+    <sheet name="Flute Butt" sheetId="2" r:id="rId2"/>
+    <sheet name="Sax Butt" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -24,7 +25,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="93">
   <si>
     <t>Button</t>
   </si>
@@ -70,9 +73,6 @@
     <t>L-thumb</t>
   </si>
   <si>
-    <t>D-0</t>
-  </si>
-  <si>
     <t>C5</t>
   </si>
   <si>
@@ -184,9 +184,6 @@
     <t>air down</t>
   </si>
   <si>
-    <t>R-Thumb</t>
-  </si>
-  <si>
     <t>R-Index</t>
   </si>
   <si>
@@ -248,6 +245,75 @@
   </si>
   <si>
     <t>Analog 1</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>Ab4</t>
+  </si>
+  <si>
+    <t>G4</t>
+  </si>
+  <si>
+    <t>Gb4</t>
+  </si>
+  <si>
+    <t>F4</t>
+  </si>
+  <si>
+    <t>E4</t>
+  </si>
+  <si>
+    <t>Eb4</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>Db4</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>Db6</t>
+  </si>
+  <si>
+    <t>D6</t>
+  </si>
+  <si>
+    <t>Eb6</t>
+  </si>
+  <si>
+    <t>E6</t>
+  </si>
+  <si>
+    <t>F6</t>
+  </si>
+  <si>
+    <t>Gb6</t>
+  </si>
+  <si>
+    <t>G6</t>
+  </si>
+  <si>
+    <t>Ab6</t>
+  </si>
+  <si>
+    <t>A6</t>
+  </si>
+  <si>
+    <t>Bb6</t>
+  </si>
+  <si>
+    <t>L-Thumb</t>
+  </si>
+  <si>
+    <t>D-10</t>
   </si>
 </sst>
 </file>
@@ -298,7 +364,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -323,8 +389,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="17">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -516,17 +588,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -552,7 +613,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -596,16 +657,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -620,19 +672,35 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -951,7 +1019,7 @@
   <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y9" sqref="Y9"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1028,7 +1096,7 @@
         <v>11</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -1047,16 +1115,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="5">
         <v>84</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -1075,16 +1143,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="5">
         <v>85</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -1103,16 +1171,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" s="5">
         <v>86</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -1131,16 +1199,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" s="5">
         <v>87</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="3"/>
@@ -1159,16 +1227,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" s="5">
         <v>88</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="3"/>
@@ -1187,16 +1255,16 @@
         <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9" s="5">
         <v>89</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="3"/>
@@ -1215,16 +1283,16 @@
         <v>8</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10" s="5">
         <v>90</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
@@ -1243,16 +1311,16 @@
         <v>9</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C11" s="5">
         <v>91</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>36</v>
+        <v>92</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
@@ -1293,7 +1361,7 @@
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G13" s="9">
         <v>1</v>
@@ -1323,19 +1391,19 @@
         <v>9</v>
       </c>
       <c r="P13" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G14" s="12">
         <v>1</v>
@@ -1375,7 +1443,7 @@
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G15" s="12">
         <v>1</v>
@@ -1415,7 +1483,7 @@
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G16" s="12">
         <v>0</v>
@@ -1455,7 +1523,7 @@
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G17" s="12">
         <v>0</v>
@@ -1495,7 +1563,7 @@
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G18" s="12">
         <v>1</v>
@@ -1535,7 +1603,7 @@
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G19" s="12">
         <v>1</v>
@@ -1575,7 +1643,7 @@
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G20" s="12">
         <v>1</v>
@@ -1615,7 +1683,7 @@
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G21" s="12">
         <v>1</v>
@@ -1655,7 +1723,7 @@
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G22" s="12">
         <v>1</v>
@@ -1695,7 +1763,7 @@
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G23" s="12">
         <v>1</v>
@@ -1735,7 +1803,7 @@
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G24" s="12">
         <v>1</v>
@@ -1775,7 +1843,7 @@
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G25" s="12">
         <v>1</v>
@@ -1815,7 +1883,7 @@
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G26" s="12">
         <v>1</v>
@@ -1856,10 +1924,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DDB5048-288C-4E27-86A5-674A8DB8F2C2}">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:N38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1869,612 +1937,1469 @@
     <col min="3" max="3" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="13" t="s">
+      <c r="E1" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="L1" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="M1" s="14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="33"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="D1" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="J1" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="K1" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="L1" s="14" t="s">
+      <c r="D2" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="E2" s="17" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="19" t="s">
+      <c r="F2" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="K2" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="M2" s="17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A3" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="32"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="20"/>
+    </row>
+    <row r="4" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="15">
+        <v>262</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="22"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
+      <c r="L4" s="27"/>
+      <c r="M4" s="27"/>
+      <c r="N4" s="30"/>
+    </row>
+    <row r="5" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="15">
+        <v>277</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="22"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="27"/>
+      <c r="L5" s="27"/>
+      <c r="M5" s="27"/>
+      <c r="N5" s="30"/>
+    </row>
+    <row r="6" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="15">
+        <v>294</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" s="22"/>
+      <c r="D6" s="24">
+        <v>0</v>
+      </c>
+      <c r="E6" s="25">
+        <v>1</v>
+      </c>
+      <c r="F6" s="25">
+        <v>1</v>
+      </c>
+      <c r="G6" s="25">
+        <v>1</v>
+      </c>
+      <c r="H6" s="25">
+        <v>1</v>
+      </c>
+      <c r="I6" s="25">
+        <v>0</v>
+      </c>
+      <c r="J6" s="25">
+        <v>1</v>
+      </c>
+      <c r="K6" s="25">
+        <v>1</v>
+      </c>
+      <c r="L6" s="25">
+        <v>1</v>
+      </c>
+      <c r="M6" s="25">
+        <v>0</v>
+      </c>
+      <c r="N6" s="30"/>
+    </row>
+    <row r="7" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="15">
+        <v>311</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="22"/>
+      <c r="D7" s="24">
+        <v>0</v>
+      </c>
+      <c r="E7" s="25">
+        <v>1</v>
+      </c>
+      <c r="F7" s="25">
+        <v>1</v>
+      </c>
+      <c r="G7" s="25">
+        <v>1</v>
+      </c>
+      <c r="H7" s="25">
+        <v>1</v>
+      </c>
+      <c r="I7" s="25">
+        <v>0</v>
+      </c>
+      <c r="J7" s="25">
+        <v>1</v>
+      </c>
+      <c r="K7" s="25">
+        <v>1</v>
+      </c>
+      <c r="L7" s="25">
+        <v>1</v>
+      </c>
+      <c r="M7" s="25">
+        <v>1</v>
+      </c>
+      <c r="N7" s="30"/>
+    </row>
+    <row r="8" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="15">
+        <v>329</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="22"/>
+      <c r="D8" s="24">
+        <v>1</v>
+      </c>
+      <c r="E8" s="25">
+        <v>1</v>
+      </c>
+      <c r="F8" s="25">
+        <v>1</v>
+      </c>
+      <c r="G8" s="25">
+        <v>1</v>
+      </c>
+      <c r="H8" s="25">
+        <v>1</v>
+      </c>
+      <c r="I8" s="25">
+        <v>0</v>
+      </c>
+      <c r="J8" s="25">
+        <v>1</v>
+      </c>
+      <c r="K8" s="25">
+        <v>1</v>
+      </c>
+      <c r="L8" s="25">
+        <v>0</v>
+      </c>
+      <c r="M8" s="25">
+        <v>1</v>
+      </c>
+      <c r="N8" s="30"/>
+    </row>
+    <row r="9" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="15">
+        <v>349</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" s="22"/>
+      <c r="D9" s="24">
+        <v>1</v>
+      </c>
+      <c r="E9" s="25">
+        <v>1</v>
+      </c>
+      <c r="F9" s="25">
+        <v>1</v>
+      </c>
+      <c r="G9" s="25">
+        <v>1</v>
+      </c>
+      <c r="H9" s="25">
+        <v>1</v>
+      </c>
+      <c r="I9" s="25">
+        <v>0</v>
+      </c>
+      <c r="J9" s="25">
+        <v>1</v>
+      </c>
+      <c r="K9" s="25">
+        <v>0</v>
+      </c>
+      <c r="L9" s="25">
+        <v>0</v>
+      </c>
+      <c r="M9" s="25">
+        <v>1</v>
+      </c>
+      <c r="N9" s="30"/>
+    </row>
+    <row r="10" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="15">
+        <v>370</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="22"/>
+      <c r="D10" s="24">
+        <v>1</v>
+      </c>
+      <c r="E10" s="25">
+        <v>1</v>
+      </c>
+      <c r="F10" s="25">
+        <v>1</v>
+      </c>
+      <c r="G10" s="25">
+        <v>1</v>
+      </c>
+      <c r="H10" s="25">
+        <v>1</v>
+      </c>
+      <c r="I10" s="25">
+        <v>0</v>
+      </c>
+      <c r="J10" s="25">
+        <v>0</v>
+      </c>
+      <c r="K10" s="25">
+        <v>0</v>
+      </c>
+      <c r="L10" s="25">
+        <v>1</v>
+      </c>
+      <c r="M10" s="25">
+        <v>1</v>
+      </c>
+      <c r="N10" s="30"/>
+    </row>
+    <row r="11" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="15">
+        <v>392</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" s="22"/>
+      <c r="D11" s="24">
+        <v>1</v>
+      </c>
+      <c r="E11" s="25">
+        <v>1</v>
+      </c>
+      <c r="F11" s="25">
+        <v>1</v>
+      </c>
+      <c r="G11" s="25">
+        <v>1</v>
+      </c>
+      <c r="H11" s="25">
+        <v>1</v>
+      </c>
+      <c r="I11" s="25">
+        <v>0</v>
+      </c>
+      <c r="J11" s="25">
+        <v>0</v>
+      </c>
+      <c r="K11" s="25">
+        <v>0</v>
+      </c>
+      <c r="L11" s="25">
+        <v>0</v>
+      </c>
+      <c r="M11" s="25">
+        <v>1</v>
+      </c>
+      <c r="N11" s="30"/>
+    </row>
+    <row r="12" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="15">
+        <v>415</v>
+      </c>
+      <c r="B12" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="D2" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="E2" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="F2" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="G2" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="H2" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="I2" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="J2" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="K2" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="L2" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="M2" s="20" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A3" s="16" t="s">
+      <c r="C12" s="22"/>
+      <c r="D12" s="24">
+        <v>1</v>
+      </c>
+      <c r="E12" s="25">
+        <v>1</v>
+      </c>
+      <c r="F12" s="25">
+        <v>1</v>
+      </c>
+      <c r="G12" s="25">
+        <v>1</v>
+      </c>
+      <c r="H12" s="25">
+        <v>1</v>
+      </c>
+      <c r="I12" s="25">
+        <v>1</v>
+      </c>
+      <c r="J12" s="25">
+        <v>0</v>
+      </c>
+      <c r="K12" s="25">
+        <v>0</v>
+      </c>
+      <c r="L12" s="25">
+        <v>0</v>
+      </c>
+      <c r="M12" s="25">
+        <v>1</v>
+      </c>
+      <c r="N12" s="30"/>
+    </row>
+    <row r="13" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="15">
+        <v>440</v>
+      </c>
+      <c r="B13" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="22"/>
-      <c r="M3" s="23"/>
-    </row>
-    <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="17">
+      <c r="C13" s="22"/>
+      <c r="D13" s="24">
+        <v>1</v>
+      </c>
+      <c r="E13" s="25">
+        <v>1</v>
+      </c>
+      <c r="F13" s="25">
+        <v>1</v>
+      </c>
+      <c r="G13" s="25">
+        <v>1</v>
+      </c>
+      <c r="H13" s="25">
+        <v>0</v>
+      </c>
+      <c r="I13" s="25">
+        <v>0</v>
+      </c>
+      <c r="J13" s="25">
+        <v>0</v>
+      </c>
+      <c r="K13" s="25">
+        <v>0</v>
+      </c>
+      <c r="L13" s="25">
+        <v>0</v>
+      </c>
+      <c r="M13" s="25">
+        <v>1</v>
+      </c>
+      <c r="N13" s="30"/>
+    </row>
+    <row r="14" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="15">
         <v>466</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B14" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="22"/>
+      <c r="D14" s="24">
+        <v>1</v>
+      </c>
+      <c r="E14" s="25">
+        <v>1</v>
+      </c>
+      <c r="F14" s="25">
+        <v>1</v>
+      </c>
+      <c r="G14" s="25">
+        <v>0</v>
+      </c>
+      <c r="H14" s="25">
+        <v>0</v>
+      </c>
+      <c r="I14" s="25">
+        <v>0</v>
+      </c>
+      <c r="J14" s="25">
+        <v>1</v>
+      </c>
+      <c r="K14" s="25">
+        <v>0</v>
+      </c>
+      <c r="L14" s="25">
+        <v>0</v>
+      </c>
+      <c r="M14" s="25">
+        <v>1</v>
+      </c>
+      <c r="N14" s="30"/>
+    </row>
+    <row r="15" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="15">
+        <v>494</v>
+      </c>
+      <c r="B15" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="25"/>
-      <c r="D4" s="27">
-        <v>0</v>
-      </c>
-      <c r="E4" s="28">
-        <v>1</v>
-      </c>
-      <c r="F4" s="28">
-        <v>1</v>
-      </c>
-      <c r="G4" s="28">
-        <v>0</v>
-      </c>
-      <c r="H4" s="28">
-        <v>0</v>
-      </c>
-      <c r="I4" s="28">
-        <v>0</v>
-      </c>
-      <c r="J4" s="28">
-        <v>1</v>
-      </c>
-      <c r="K4" s="28">
-        <v>0</v>
-      </c>
-      <c r="L4" s="28">
-        <v>0</v>
-      </c>
-      <c r="M4" s="28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="17">
-        <v>494</v>
-      </c>
-      <c r="B5" s="24" t="s">
+      <c r="C15" s="22"/>
+      <c r="D15" s="28">
+        <v>1</v>
+      </c>
+      <c r="E15" s="29">
+        <v>1</v>
+      </c>
+      <c r="F15" s="29">
+        <v>1</v>
+      </c>
+      <c r="G15" s="29">
+        <v>0</v>
+      </c>
+      <c r="H15" s="29">
+        <v>0</v>
+      </c>
+      <c r="I15" s="29">
+        <v>0</v>
+      </c>
+      <c r="J15" s="29">
+        <v>0</v>
+      </c>
+      <c r="K15" s="29">
+        <v>0</v>
+      </c>
+      <c r="L15" s="29">
+        <v>0</v>
+      </c>
+      <c r="M15" s="29">
+        <v>1</v>
+      </c>
+      <c r="N15" s="30"/>
+    </row>
+    <row r="16" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="15">
+        <v>523</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="22"/>
+      <c r="D16" s="28">
+        <v>1</v>
+      </c>
+      <c r="E16" s="29">
+        <v>0</v>
+      </c>
+      <c r="F16" s="29">
+        <v>1</v>
+      </c>
+      <c r="G16" s="29">
+        <v>0</v>
+      </c>
+      <c r="H16" s="29">
+        <v>0</v>
+      </c>
+      <c r="I16" s="29">
+        <v>0</v>
+      </c>
+      <c r="J16" s="29">
+        <v>0</v>
+      </c>
+      <c r="K16" s="29">
+        <v>0</v>
+      </c>
+      <c r="L16" s="29">
+        <v>0</v>
+      </c>
+      <c r="M16" s="29">
+        <v>1</v>
+      </c>
+      <c r="N16" s="30"/>
+    </row>
+    <row r="17" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="15">
+        <v>554</v>
+      </c>
+      <c r="B17" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="25"/>
-      <c r="D5" s="29">
-        <v>0</v>
-      </c>
-      <c r="E5" s="30">
-        <v>1</v>
-      </c>
-      <c r="F5" s="30">
-        <v>1</v>
-      </c>
-      <c r="G5" s="30">
-        <v>0</v>
-      </c>
-      <c r="H5" s="30">
-        <v>0</v>
-      </c>
-      <c r="I5" s="30">
-        <v>0</v>
-      </c>
-      <c r="J5" s="30">
-        <v>0</v>
-      </c>
-      <c r="K5" s="30">
-        <v>0</v>
-      </c>
-      <c r="L5" s="30">
-        <v>0</v>
-      </c>
-      <c r="M5" s="30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="17">
-        <v>523</v>
-      </c>
-      <c r="B6" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="29">
-        <v>0</v>
-      </c>
-      <c r="E6" s="30">
-        <v>0</v>
-      </c>
-      <c r="F6" s="30">
-        <v>1</v>
-      </c>
-      <c r="G6" s="30">
-        <v>0</v>
-      </c>
-      <c r="H6" s="30">
-        <v>0</v>
-      </c>
-      <c r="I6" s="30">
-        <v>0</v>
-      </c>
-      <c r="J6" s="30">
-        <v>0</v>
-      </c>
-      <c r="K6" s="30">
-        <v>0</v>
-      </c>
-      <c r="L6" s="30">
-        <v>0</v>
-      </c>
-      <c r="M6" s="30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="17">
-        <v>554</v>
-      </c>
-      <c r="B7" s="24" t="s">
+      <c r="C17" s="22"/>
+      <c r="D17" s="28">
+        <v>1</v>
+      </c>
+      <c r="E17" s="29">
+        <v>0</v>
+      </c>
+      <c r="F17" s="29">
+        <v>0</v>
+      </c>
+      <c r="G17" s="29">
+        <v>0</v>
+      </c>
+      <c r="H17" s="29">
+        <v>0</v>
+      </c>
+      <c r="I17" s="29">
+        <v>0</v>
+      </c>
+      <c r="J17" s="29">
+        <v>0</v>
+      </c>
+      <c r="K17" s="29">
+        <v>0</v>
+      </c>
+      <c r="L17" s="29">
+        <v>0</v>
+      </c>
+      <c r="M17" s="29">
+        <v>1</v>
+      </c>
+      <c r="N17" s="30"/>
+    </row>
+    <row r="18" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="15">
+        <v>587</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="22"/>
+      <c r="D18" s="28">
+        <v>0</v>
+      </c>
+      <c r="E18" s="29">
+        <v>1</v>
+      </c>
+      <c r="F18" s="29">
+        <v>0</v>
+      </c>
+      <c r="G18" s="29">
+        <v>1</v>
+      </c>
+      <c r="H18" s="29">
+        <v>1</v>
+      </c>
+      <c r="I18" s="29">
+        <v>0</v>
+      </c>
+      <c r="J18" s="29">
+        <v>1</v>
+      </c>
+      <c r="K18" s="29">
+        <v>1</v>
+      </c>
+      <c r="L18" s="29">
+        <v>1</v>
+      </c>
+      <c r="M18" s="29">
+        <v>0</v>
+      </c>
+      <c r="N18" s="30"/>
+    </row>
+    <row r="19" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="15">
+        <v>622</v>
+      </c>
+      <c r="B19" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="29">
-        <v>0</v>
-      </c>
-      <c r="E7" s="30">
-        <v>0</v>
-      </c>
-      <c r="F7" s="30">
-        <v>0</v>
-      </c>
-      <c r="G7" s="30">
-        <v>0</v>
-      </c>
-      <c r="H7" s="30">
-        <v>0</v>
-      </c>
-      <c r="I7" s="30">
-        <v>0</v>
-      </c>
-      <c r="J7" s="30">
-        <v>0</v>
-      </c>
-      <c r="K7" s="30">
-        <v>0</v>
-      </c>
-      <c r="L7" s="30">
-        <v>0</v>
-      </c>
-      <c r="M7" s="30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="17">
-        <v>587</v>
-      </c>
-      <c r="B8" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="25"/>
-      <c r="D8" s="29">
-        <v>0</v>
-      </c>
-      <c r="E8" s="30">
-        <v>1</v>
-      </c>
-      <c r="F8" s="30">
-        <v>0</v>
-      </c>
-      <c r="G8" s="30">
-        <v>1</v>
-      </c>
-      <c r="H8" s="30">
-        <v>1</v>
-      </c>
-      <c r="I8" s="30">
-        <v>0</v>
-      </c>
-      <c r="J8" s="30">
-        <v>1</v>
-      </c>
-      <c r="K8" s="30">
-        <v>1</v>
-      </c>
-      <c r="L8" s="30">
-        <v>1</v>
-      </c>
-      <c r="M8" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="17">
-        <v>622</v>
-      </c>
-      <c r="B9" s="24" t="s">
+      <c r="C19" s="22"/>
+      <c r="D19" s="28">
+        <v>0</v>
+      </c>
+      <c r="E19" s="29">
+        <v>1</v>
+      </c>
+      <c r="F19" s="29">
+        <v>0</v>
+      </c>
+      <c r="G19" s="29">
+        <v>1</v>
+      </c>
+      <c r="H19" s="29">
+        <v>1</v>
+      </c>
+      <c r="I19" s="29">
+        <v>0</v>
+      </c>
+      <c r="J19" s="29">
+        <v>1</v>
+      </c>
+      <c r="K19" s="29">
+        <v>1</v>
+      </c>
+      <c r="L19" s="29">
+        <v>1</v>
+      </c>
+      <c r="M19" s="29">
+        <v>1</v>
+      </c>
+      <c r="N19" s="30"/>
+    </row>
+    <row r="20" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="15">
+        <v>659</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="22"/>
+      <c r="D20" s="28">
+        <v>0</v>
+      </c>
+      <c r="E20" s="29">
+        <v>1</v>
+      </c>
+      <c r="F20" s="29">
+        <v>1</v>
+      </c>
+      <c r="G20" s="29">
+        <v>1</v>
+      </c>
+      <c r="H20" s="29">
+        <v>1</v>
+      </c>
+      <c r="I20" s="29">
+        <v>0</v>
+      </c>
+      <c r="J20" s="29">
+        <v>1</v>
+      </c>
+      <c r="K20" s="29">
+        <v>1</v>
+      </c>
+      <c r="L20" s="29">
+        <v>0</v>
+      </c>
+      <c r="M20" s="29">
+        <v>1</v>
+      </c>
+      <c r="N20" s="30"/>
+    </row>
+    <row r="21" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="15">
+        <v>698</v>
+      </c>
+      <c r="B21" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="22"/>
+      <c r="D21" s="28">
+        <v>0</v>
+      </c>
+      <c r="E21" s="29">
+        <v>1</v>
+      </c>
+      <c r="F21" s="29">
+        <v>1</v>
+      </c>
+      <c r="G21" s="29">
+        <v>1</v>
+      </c>
+      <c r="H21" s="29">
+        <v>1</v>
+      </c>
+      <c r="I21" s="29">
+        <v>0</v>
+      </c>
+      <c r="J21" s="29">
+        <v>1</v>
+      </c>
+      <c r="K21" s="29">
+        <v>0</v>
+      </c>
+      <c r="L21" s="29">
+        <v>0</v>
+      </c>
+      <c r="M21" s="29">
+        <v>1</v>
+      </c>
+      <c r="N21" s="30"/>
+    </row>
+    <row r="22" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="15">
+        <v>740</v>
+      </c>
+      <c r="B22" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="29">
-        <v>0</v>
-      </c>
-      <c r="E9" s="30">
-        <v>1</v>
-      </c>
-      <c r="F9" s="30">
-        <v>0</v>
-      </c>
-      <c r="G9" s="30">
-        <v>1</v>
-      </c>
-      <c r="H9" s="30">
-        <v>1</v>
-      </c>
-      <c r="I9" s="30">
-        <v>0</v>
-      </c>
-      <c r="J9" s="30">
-        <v>1</v>
-      </c>
-      <c r="K9" s="30">
-        <v>1</v>
-      </c>
-      <c r="L9" s="30">
-        <v>1</v>
-      </c>
-      <c r="M9" s="30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="17">
-        <v>659</v>
-      </c>
-      <c r="B10" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="25"/>
-      <c r="D10" s="29">
-        <v>0</v>
-      </c>
-      <c r="E10" s="30">
-        <v>1</v>
-      </c>
-      <c r="F10" s="30">
-        <v>1</v>
-      </c>
-      <c r="G10" s="30">
-        <v>1</v>
-      </c>
-      <c r="H10" s="30">
-        <v>1</v>
-      </c>
-      <c r="I10" s="30">
-        <v>0</v>
-      </c>
-      <c r="J10" s="30">
-        <v>1</v>
-      </c>
-      <c r="K10" s="30">
-        <v>1</v>
-      </c>
-      <c r="L10" s="30">
-        <v>0</v>
-      </c>
-      <c r="M10" s="30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="17">
-        <v>698</v>
-      </c>
-      <c r="B11" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="25"/>
-      <c r="D11" s="29">
-        <v>0</v>
-      </c>
-      <c r="E11" s="30">
-        <v>1</v>
-      </c>
-      <c r="F11" s="30">
-        <v>1</v>
-      </c>
-      <c r="G11" s="30">
-        <v>1</v>
-      </c>
-      <c r="H11" s="30">
-        <v>1</v>
-      </c>
-      <c r="I11" s="30">
-        <v>0</v>
-      </c>
-      <c r="J11" s="30">
-        <v>1</v>
-      </c>
-      <c r="K11" s="30">
-        <v>0</v>
-      </c>
-      <c r="L11" s="30">
-        <v>0</v>
-      </c>
-      <c r="M11" s="30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="17">
-        <v>740</v>
-      </c>
-      <c r="B12" s="24" t="s">
+      <c r="C22" s="22"/>
+      <c r="D22" s="28">
+        <v>0</v>
+      </c>
+      <c r="E22" s="29">
+        <v>1</v>
+      </c>
+      <c r="F22" s="29">
+        <v>1</v>
+      </c>
+      <c r="G22" s="29">
+        <v>1</v>
+      </c>
+      <c r="H22" s="29">
+        <v>1</v>
+      </c>
+      <c r="I22" s="29">
+        <v>0</v>
+      </c>
+      <c r="J22" s="29">
+        <v>0</v>
+      </c>
+      <c r="K22" s="29">
+        <v>0</v>
+      </c>
+      <c r="L22" s="29">
+        <v>1</v>
+      </c>
+      <c r="M22" s="29">
+        <v>1</v>
+      </c>
+      <c r="N22" s="30"/>
+    </row>
+    <row r="23" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="15">
+        <v>784</v>
+      </c>
+      <c r="B23" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="22"/>
+      <c r="D23" s="28">
+        <v>0</v>
+      </c>
+      <c r="E23" s="29">
+        <v>1</v>
+      </c>
+      <c r="F23" s="29">
+        <v>1</v>
+      </c>
+      <c r="G23" s="29">
+        <v>1</v>
+      </c>
+      <c r="H23" s="29">
+        <v>1</v>
+      </c>
+      <c r="I23" s="29">
+        <v>0</v>
+      </c>
+      <c r="J23" s="29">
+        <v>0</v>
+      </c>
+      <c r="K23" s="29">
+        <v>0</v>
+      </c>
+      <c r="L23" s="29">
+        <v>0</v>
+      </c>
+      <c r="M23" s="29">
+        <v>1</v>
+      </c>
+      <c r="N23" s="30"/>
+    </row>
+    <row r="24" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="15">
+        <v>831</v>
+      </c>
+      <c r="B24" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="29">
-        <v>0</v>
-      </c>
-      <c r="E12" s="30">
-        <v>1</v>
-      </c>
-      <c r="F12" s="30">
-        <v>1</v>
-      </c>
-      <c r="G12" s="30">
-        <v>1</v>
-      </c>
-      <c r="H12" s="30">
-        <v>1</v>
-      </c>
-      <c r="I12" s="30">
-        <v>0</v>
-      </c>
-      <c r="J12" s="30">
-        <v>0</v>
-      </c>
-      <c r="K12" s="30">
-        <v>0</v>
-      </c>
-      <c r="L12" s="30">
-        <v>1</v>
-      </c>
-      <c r="M12" s="30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="17">
-        <v>784</v>
-      </c>
-      <c r="B13" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="25"/>
-      <c r="D13" s="29">
-        <v>0</v>
-      </c>
-      <c r="E13" s="30">
-        <v>1</v>
-      </c>
-      <c r="F13" s="30">
-        <v>1</v>
-      </c>
-      <c r="G13" s="30">
-        <v>1</v>
-      </c>
-      <c r="H13" s="30">
-        <v>1</v>
-      </c>
-      <c r="I13" s="30">
-        <v>0</v>
-      </c>
-      <c r="J13" s="30">
-        <v>0</v>
-      </c>
-      <c r="K13" s="30">
-        <v>0</v>
-      </c>
-      <c r="L13" s="30">
-        <v>0</v>
-      </c>
-      <c r="M13" s="30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="17">
-        <v>831</v>
-      </c>
-      <c r="B14" s="24" t="s">
+      <c r="C24" s="22"/>
+      <c r="D24" s="28">
+        <v>0</v>
+      </c>
+      <c r="E24" s="29">
+        <v>1</v>
+      </c>
+      <c r="F24" s="29">
+        <v>1</v>
+      </c>
+      <c r="G24" s="29">
+        <v>1</v>
+      </c>
+      <c r="H24" s="29">
+        <v>1</v>
+      </c>
+      <c r="I24" s="29">
+        <v>1</v>
+      </c>
+      <c r="J24" s="29">
+        <v>0</v>
+      </c>
+      <c r="K24" s="29">
+        <v>0</v>
+      </c>
+      <c r="L24" s="29">
+        <v>0</v>
+      </c>
+      <c r="M24" s="29">
+        <v>1</v>
+      </c>
+      <c r="N24" s="30"/>
+    </row>
+    <row r="25" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="15">
+        <v>880</v>
+      </c>
+      <c r="B25" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="25"/>
-      <c r="D14" s="29">
-        <v>0</v>
-      </c>
-      <c r="E14" s="30">
-        <v>1</v>
-      </c>
-      <c r="F14" s="30">
-        <v>1</v>
-      </c>
-      <c r="G14" s="30">
-        <v>1</v>
-      </c>
-      <c r="H14" s="30">
-        <v>1</v>
-      </c>
-      <c r="I14" s="30">
-        <v>1</v>
-      </c>
-      <c r="J14" s="30">
-        <v>0</v>
-      </c>
-      <c r="K14" s="30">
-        <v>0</v>
-      </c>
-      <c r="L14" s="30">
-        <v>0</v>
-      </c>
-      <c r="M14" s="30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="17">
-        <v>880</v>
-      </c>
-      <c r="B15" s="24" t="s">
+      <c r="C25" s="22"/>
+      <c r="D25" s="28">
+        <v>0</v>
+      </c>
+      <c r="E25" s="29">
+        <v>1</v>
+      </c>
+      <c r="F25" s="29">
+        <v>1</v>
+      </c>
+      <c r="G25" s="29">
+        <v>1</v>
+      </c>
+      <c r="H25" s="29">
+        <v>0</v>
+      </c>
+      <c r="I25" s="29">
+        <v>0</v>
+      </c>
+      <c r="J25" s="29">
+        <v>0</v>
+      </c>
+      <c r="K25" s="29">
+        <v>0</v>
+      </c>
+      <c r="L25" s="29">
+        <v>0</v>
+      </c>
+      <c r="M25" s="29">
+        <v>1</v>
+      </c>
+      <c r="N25" s="30"/>
+    </row>
+    <row r="26" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="15">
+        <v>932</v>
+      </c>
+      <c r="B26" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="25"/>
-      <c r="D15" s="29">
-        <v>0</v>
-      </c>
-      <c r="E15" s="30">
-        <v>1</v>
-      </c>
-      <c r="F15" s="30">
-        <v>1</v>
-      </c>
-      <c r="G15" s="30">
-        <v>1</v>
-      </c>
-      <c r="H15" s="30">
-        <v>0</v>
-      </c>
-      <c r="I15" s="30">
-        <v>0</v>
-      </c>
-      <c r="J15" s="30">
-        <v>0</v>
-      </c>
-      <c r="K15" s="30">
-        <v>0</v>
-      </c>
-      <c r="L15" s="30">
-        <v>0</v>
-      </c>
-      <c r="M15" s="30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="17">
-        <v>932</v>
-      </c>
-      <c r="B16" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" s="21"/>
-      <c r="D16" s="29">
-        <v>0</v>
-      </c>
-      <c r="E16" s="30">
-        <v>1</v>
-      </c>
-      <c r="F16" s="30">
-        <v>1</v>
-      </c>
-      <c r="G16" s="30">
-        <v>0</v>
-      </c>
-      <c r="H16" s="30">
-        <v>0</v>
-      </c>
-      <c r="I16" s="30">
-        <v>0</v>
-      </c>
-      <c r="J16" s="30">
-        <v>1</v>
-      </c>
-      <c r="K16" s="30">
-        <v>0</v>
-      </c>
-      <c r="L16" s="30">
-        <v>0</v>
-      </c>
-      <c r="M16" s="30">
-        <v>1</v>
-      </c>
+      <c r="C26" s="22"/>
+      <c r="D26" s="28">
+        <v>0</v>
+      </c>
+      <c r="E26" s="29">
+        <v>1</v>
+      </c>
+      <c r="F26" s="29">
+        <v>1</v>
+      </c>
+      <c r="G26" s="29">
+        <v>0</v>
+      </c>
+      <c r="H26" s="29">
+        <v>0</v>
+      </c>
+      <c r="I26" s="29">
+        <v>0</v>
+      </c>
+      <c r="J26" s="29">
+        <v>1</v>
+      </c>
+      <c r="K26" s="29">
+        <v>0</v>
+      </c>
+      <c r="L26" s="29">
+        <v>0</v>
+      </c>
+      <c r="M26" s="29">
+        <v>1</v>
+      </c>
+      <c r="N26" s="30"/>
+    </row>
+    <row r="27" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="15">
+        <v>988</v>
+      </c>
+      <c r="B27" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="22"/>
+      <c r="D27" s="28">
+        <v>0</v>
+      </c>
+      <c r="E27" s="29">
+        <v>1</v>
+      </c>
+      <c r="F27" s="29">
+        <v>1</v>
+      </c>
+      <c r="G27" s="29">
+        <v>0</v>
+      </c>
+      <c r="H27" s="29">
+        <v>0</v>
+      </c>
+      <c r="I27" s="29">
+        <v>0</v>
+      </c>
+      <c r="J27" s="29">
+        <v>0</v>
+      </c>
+      <c r="K27" s="29">
+        <v>0</v>
+      </c>
+      <c r="L27" s="29">
+        <v>0</v>
+      </c>
+      <c r="M27" s="29">
+        <v>1</v>
+      </c>
+      <c r="N27" s="30"/>
+    </row>
+    <row r="28" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="15">
+        <v>1046</v>
+      </c>
+      <c r="B28" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="C28" s="22"/>
+      <c r="D28" s="24">
+        <v>0</v>
+      </c>
+      <c r="E28" s="25">
+        <v>0</v>
+      </c>
+      <c r="F28" s="25">
+        <v>1</v>
+      </c>
+      <c r="G28" s="25">
+        <v>0</v>
+      </c>
+      <c r="H28" s="25">
+        <v>0</v>
+      </c>
+      <c r="I28" s="25">
+        <v>0</v>
+      </c>
+      <c r="J28" s="25">
+        <v>0</v>
+      </c>
+      <c r="K28" s="25">
+        <v>0</v>
+      </c>
+      <c r="L28" s="25">
+        <v>0</v>
+      </c>
+      <c r="M28" s="25">
+        <v>1</v>
+      </c>
+      <c r="N28" s="30"/>
+    </row>
+    <row r="29" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="15">
+        <v>1108</v>
+      </c>
+      <c r="B29" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="C29" s="22"/>
+      <c r="D29" s="24">
+        <v>0</v>
+      </c>
+      <c r="E29" s="25">
+        <v>0</v>
+      </c>
+      <c r="F29" s="25">
+        <v>0</v>
+      </c>
+      <c r="G29" s="25">
+        <v>0</v>
+      </c>
+      <c r="H29" s="25">
+        <v>0</v>
+      </c>
+      <c r="I29" s="25">
+        <v>0</v>
+      </c>
+      <c r="J29" s="25">
+        <v>0</v>
+      </c>
+      <c r="K29" s="25">
+        <v>0</v>
+      </c>
+      <c r="L29" s="25">
+        <v>0</v>
+      </c>
+      <c r="M29" s="25">
+        <v>1</v>
+      </c>
+      <c r="N29" s="30"/>
+    </row>
+    <row r="30" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="15">
+        <v>1174</v>
+      </c>
+      <c r="B30" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="C30" s="22"/>
+      <c r="D30" s="24">
+        <v>0</v>
+      </c>
+      <c r="E30" s="25">
+        <v>1</v>
+      </c>
+      <c r="F30" s="25">
+        <v>0</v>
+      </c>
+      <c r="G30" s="25">
+        <v>1</v>
+      </c>
+      <c r="H30" s="25">
+        <v>1</v>
+      </c>
+      <c r="I30" s="25">
+        <v>0</v>
+      </c>
+      <c r="J30" s="25">
+        <v>0</v>
+      </c>
+      <c r="K30" s="25">
+        <v>0</v>
+      </c>
+      <c r="L30" s="25">
+        <v>0</v>
+      </c>
+      <c r="M30" s="25">
+        <v>1</v>
+      </c>
+      <c r="N30" s="30"/>
+    </row>
+    <row r="31" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="15">
+        <v>1245</v>
+      </c>
+      <c r="B31" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="C31" s="22"/>
+      <c r="D31" s="24">
+        <v>0</v>
+      </c>
+      <c r="E31" s="25">
+        <v>1</v>
+      </c>
+      <c r="F31" s="25">
+        <v>1</v>
+      </c>
+      <c r="G31" s="25">
+        <v>1</v>
+      </c>
+      <c r="H31" s="25">
+        <v>1</v>
+      </c>
+      <c r="I31" s="25">
+        <v>1</v>
+      </c>
+      <c r="J31" s="25">
+        <v>1</v>
+      </c>
+      <c r="K31" s="25">
+        <v>1</v>
+      </c>
+      <c r="L31" s="25">
+        <v>1</v>
+      </c>
+      <c r="M31" s="25">
+        <v>1</v>
+      </c>
+      <c r="N31" s="30"/>
+    </row>
+    <row r="32" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="15">
+        <v>1319</v>
+      </c>
+      <c r="B32" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32" s="22"/>
+      <c r="D32" s="24">
+        <v>0</v>
+      </c>
+      <c r="E32" s="25">
+        <v>1</v>
+      </c>
+      <c r="F32" s="25">
+        <v>1</v>
+      </c>
+      <c r="G32" s="25">
+        <v>1</v>
+      </c>
+      <c r="H32" s="25">
+        <v>0</v>
+      </c>
+      <c r="I32" s="25">
+        <v>0</v>
+      </c>
+      <c r="J32" s="25">
+        <v>1</v>
+      </c>
+      <c r="K32" s="25">
+        <v>1</v>
+      </c>
+      <c r="L32" s="25">
+        <v>0</v>
+      </c>
+      <c r="M32" s="25">
+        <v>1</v>
+      </c>
+      <c r="N32" s="30"/>
+    </row>
+    <row r="33" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="15">
+        <v>1397</v>
+      </c>
+      <c r="B33" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="C33" s="22"/>
+      <c r="D33" s="24">
+        <v>0</v>
+      </c>
+      <c r="E33" s="25">
+        <v>1</v>
+      </c>
+      <c r="F33" s="25">
+        <v>1</v>
+      </c>
+      <c r="G33" s="25">
+        <v>0</v>
+      </c>
+      <c r="H33" s="25">
+        <v>1</v>
+      </c>
+      <c r="I33" s="25">
+        <v>0</v>
+      </c>
+      <c r="J33" s="25">
+        <v>1</v>
+      </c>
+      <c r="K33" s="25">
+        <v>0</v>
+      </c>
+      <c r="L33" s="25">
+        <v>0</v>
+      </c>
+      <c r="M33" s="25">
+        <v>1</v>
+      </c>
+      <c r="N33" s="30"/>
+    </row>
+    <row r="34" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="15">
+        <v>1480</v>
+      </c>
+      <c r="B34" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="C34" s="22"/>
+      <c r="D34" s="24">
+        <v>0</v>
+      </c>
+      <c r="E34" s="25">
+        <v>1</v>
+      </c>
+      <c r="F34" s="25">
+        <v>1</v>
+      </c>
+      <c r="G34" s="25">
+        <v>0</v>
+      </c>
+      <c r="H34" s="25">
+        <v>1</v>
+      </c>
+      <c r="I34" s="25">
+        <v>0</v>
+      </c>
+      <c r="J34" s="25">
+        <v>0</v>
+      </c>
+      <c r="K34" s="25">
+        <v>0</v>
+      </c>
+      <c r="L34" s="25">
+        <v>1</v>
+      </c>
+      <c r="M34" s="25">
+        <v>1</v>
+      </c>
+      <c r="N34" s="30"/>
+    </row>
+    <row r="35" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="15">
+        <v>1568</v>
+      </c>
+      <c r="B35" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="C35" s="22"/>
+      <c r="D35" s="24">
+        <v>0</v>
+      </c>
+      <c r="E35" s="25">
+        <v>0</v>
+      </c>
+      <c r="F35" s="25">
+        <v>1</v>
+      </c>
+      <c r="G35" s="25">
+        <v>1</v>
+      </c>
+      <c r="H35" s="25">
+        <v>1</v>
+      </c>
+      <c r="I35" s="25">
+        <v>0</v>
+      </c>
+      <c r="J35" s="25">
+        <v>0</v>
+      </c>
+      <c r="K35" s="25">
+        <v>0</v>
+      </c>
+      <c r="L35" s="25">
+        <v>0</v>
+      </c>
+      <c r="M35" s="25">
+        <v>1</v>
+      </c>
+      <c r="N35" s="30"/>
+    </row>
+    <row r="36" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="15">
+        <v>1661</v>
+      </c>
+      <c r="B36" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C36" s="22"/>
+      <c r="D36" s="24">
+        <v>0</v>
+      </c>
+      <c r="E36" s="25">
+        <v>0</v>
+      </c>
+      <c r="F36" s="25">
+        <v>0</v>
+      </c>
+      <c r="G36" s="25">
+        <v>1</v>
+      </c>
+      <c r="H36" s="25">
+        <v>1</v>
+      </c>
+      <c r="I36" s="25">
+        <v>1</v>
+      </c>
+      <c r="J36" s="25">
+        <v>0</v>
+      </c>
+      <c r="K36" s="25">
+        <v>0</v>
+      </c>
+      <c r="L36" s="25">
+        <v>0</v>
+      </c>
+      <c r="M36" s="25">
+        <v>1</v>
+      </c>
+      <c r="N36" s="30"/>
+    </row>
+    <row r="37" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="15">
+        <v>1760</v>
+      </c>
+      <c r="B37" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="C37" s="22"/>
+      <c r="D37" s="24">
+        <v>0</v>
+      </c>
+      <c r="E37" s="25">
+        <v>1</v>
+      </c>
+      <c r="F37" s="25">
+        <v>0</v>
+      </c>
+      <c r="G37" s="25">
+        <v>1</v>
+      </c>
+      <c r="H37" s="25">
+        <v>0</v>
+      </c>
+      <c r="I37" s="25">
+        <v>0</v>
+      </c>
+      <c r="J37" s="25">
+        <v>1</v>
+      </c>
+      <c r="K37" s="25">
+        <v>0</v>
+      </c>
+      <c r="L37" s="25">
+        <v>0</v>
+      </c>
+      <c r="M37" s="25">
+        <v>1</v>
+      </c>
+      <c r="N37" s="30"/>
+    </row>
+    <row r="38" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="15">
+        <v>1865</v>
+      </c>
+      <c r="B38" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="C38" s="18"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="27"/>
+      <c r="F38" s="27"/>
+      <c r="G38" s="27"/>
+      <c r="H38" s="27"/>
+      <c r="I38" s="27"/>
+      <c r="J38" s="27"/>
+      <c r="K38" s="27"/>
+      <c r="L38" s="27"/>
+      <c r="M38" s="27"/>
+      <c r="N38" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A1:B2"/>
   </mergeCells>
+  <conditionalFormatting sqref="D6:M37">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9C07B39-7804-4172-941C-A931A11BEE0F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>